<commit_message>
Support multi-target upgrades with percent attack bonuses
</commit_message>
<xml_diff>
--- a/war3_units_full.xlsx
+++ b/war3_units_full.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Orc" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Human" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NightElf" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Undead" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Orc" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Human" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="NightElf" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Undead" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1117,6 +1117,58 @@
       <c r="N13" t="inlineStr">
         <is>
           <t>Light</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Demolisher</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>220</v>
+      </c>
+      <c r="C14" t="n">
+        <v>50</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>45</v>
+      </c>
+      <c r="F14" t="n">
+        <v>72</v>
+      </c>
+      <c r="G14" t="n">
+        <v>89</v>
+      </c>
+      <c r="H14" t="n">
+        <v>425</v>
+      </c>
+      <c r="I14" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" t="n">
+        <v>600</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Siege</t>
+        </is>
+      </c>
+      <c r="L14" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>Siege</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Heavy</t>
         </is>
       </c>
     </row>
@@ -1791,7 +1843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2440,6 +2492,58 @@
       <c r="N12" t="inlineStr">
         <is>
           <t>Heavy</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Mountain Giant</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>350</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="n">
+        <v>60</v>
+      </c>
+      <c r="F13" t="n">
+        <v>28</v>
+      </c>
+      <c r="G13" t="n">
+        <v>40</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1600</v>
+      </c>
+      <c r="I13" t="n">
+        <v>6</v>
+      </c>
+      <c r="J13" t="n">
+        <v>100</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Melee</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Medium</t>
         </is>
       </c>
     </row>
@@ -2454,7 +2558,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3054,6 +3158,58 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Obsidian Statue</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>200</v>
+      </c>
+      <c r="C12" t="n">
+        <v>35</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8</v>
+      </c>
+      <c r="H12" t="n">
+        <v>500</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="n">
+        <v>575</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Ranged</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>Magic</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Heavy</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>